<commit_message>
Added another version of testin
</commit_message>
<xml_diff>
--- a/Documentation/Request_Data_Details.xlsx
+++ b/Documentation/Request_Data_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65D1442-3FD0-404C-A879-0D024AEE95E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D955B302-6E50-4A8C-A0C5-645ADE23C3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,8 +1094,8 @@
   </sheetPr>
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>